<commit_message>
Prepare X and y from incident and factor df Re-shape the factors dataframe in a way that it can create the X and y as input for modelling
</commit_message>
<xml_diff>
--- a/out/factors_3.xlsx
+++ b/out/factors_3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,59 +702,59 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>assignment_group_company</t>
+          <t>close_code_No Resolution Action</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>analysis2</t>
+          <t>analyse</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>uint8</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>108.405148086512</v>
+        <v>212.5657420134024</v>
       </c>
       <c r="F11" t="n">
-        <v>3.104338295130162e-19</v>
+        <v>3.785379350270401e-48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>priority_is_4</t>
+          <t>assignment_group_company</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>analyse</t>
+          <t>analyse2</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>object</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>103.8263314178949</v>
+        <v>108.405148086512</v>
       </c>
       <c r="F12" t="n">
-        <v>2.208504274319012e-24</v>
+        <v>3.104338295130162e-19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>caller_is_employee</t>
+          <t>close_code_Data Correction</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -764,28 +764,28 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>uint8</t>
         </is>
       </c>
       <c r="D13" t="n">
         <v>2</v>
       </c>
       <c r="E13" t="n">
-        <v>89.71333796111035</v>
+        <v>103.9629160967067</v>
       </c>
       <c r="F13" t="n">
-        <v>2.752927944834831e-21</v>
+        <v>2.061384633699008e-24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ka_count_log</t>
+          <t>priority_is_4</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ignore</t>
+          <t>analyse</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -794,45 +794,45 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>69.71864170960302</v>
+        <v>103.8263314178949</v>
       </c>
       <c r="F14" t="n">
-        <v>5.590814295923098e-12</v>
+        <v>2.208504274319012e-24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>contact_type</t>
+          <t>caller_is_employee</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ignore</t>
+          <t>analyse</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>62.83893362299189</v>
+        <v>89.71333796111035</v>
       </c>
       <c r="F15" t="n">
-        <v>7.336768356839108e-13</v>
+        <v>2.752927944834831e-21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>breached_reason_code</t>
+          <t>ka_count_log</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -842,106 +842,106 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E16" t="n">
-        <v>55.22842804766915</v>
+        <v>69.71864170960302</v>
       </c>
       <c r="F16" t="n">
-        <v>1.647005452924161e-07</v>
+        <v>5.590814295923098e-12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>incident_has_ka_related_flag</t>
+          <t>contact_type</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>analyse</t>
+          <t>ignore</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>object</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E17" t="n">
-        <v>38.95749777616205</v>
+        <v>62.83893362299189</v>
       </c>
       <c r="F17" t="n">
-        <v>4.33133544018824e-10</v>
+        <v>7.336768356839108e-13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>self_service</t>
+          <t>breached_reason_code</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>analyse</t>
+          <t>ignore</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>object</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E18" t="n">
-        <v>31.27813668428506</v>
+        <v>55.22842804766915</v>
       </c>
       <c r="F18" t="n">
-        <v>2.23583427847182e-08</v>
+        <v>1.647005452924161e-07</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>appl_tier</t>
+          <t>incident_has_ka_related_flag</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ignore</t>
+          <t>analyse</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>int64</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>27.66288814486726</v>
+        <v>38.95749777616205</v>
       </c>
       <c r="F19" t="n">
-        <v>4.274586770349934e-06</v>
+        <v>4.33133544018824e-10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>caller_vip</t>
+          <t>self_service</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ignore</t>
+          <t>analyse</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -953,33 +953,215 @@
         <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2128688205425569</v>
+        <v>31.27813668428506</v>
       </c>
       <c r="F20" t="n">
-        <v>0.644528084295426</v>
+        <v>2.23583427847182e-08</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>close_code_Reboot / Restart</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>analyse</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>uint8</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="n">
+        <v>29.17596056897717</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6.609418315501527e-08</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>appl_tier</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ignore</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>object</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" t="n">
+        <v>27.66288814486726</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4.274586770349934e-06</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>close_code_Security Modification</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>analyse</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>uint8</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="n">
+        <v>21.3501624171497</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3.825883411918223e-06</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>close_code_Software Correction</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>analyse</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>uint8</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12.15795061766993</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0004887905515663779</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>close_code_Environmental Restoration</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>analyse</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>uint8</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.50656659638963</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.06112600893982762</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>close_code_Information Provided / Training</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>analyse</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>uint8</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.3786840534703145</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.538308351370397</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>caller_vip</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ignore</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>int64</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.2128688205425569</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.644528084295426</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>user_dissatisfied</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>response</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>int64</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>